<commit_message>
Set up geo zones,tax rates & weight based shipping
</commit_message>
<xml_diff>
--- a/change-status-of-usa-and-europe-countries-in-country-table-via-mysql.xlsx
+++ b/change-status-of-usa-and-europe-countries-in-country-table-via-mysql.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="202">
   <si>
     <t>Albania</t>
   </si>
@@ -470,6 +470,156 @@
   </si>
   <si>
     <t>;</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='AL';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='AD';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='AM';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='AT';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='AZ';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='BY';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='BE';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='BA';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='BG';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='HR';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='CZ';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='DK';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='EE';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='FI';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='FR';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='GE';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='DE';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='GR';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='HU';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='IS';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='IE';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='IT';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='KZ';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='LV';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='LI';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='LT';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='LU';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='MT';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='MD';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='MC';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='NL';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='NO';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='PL';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='PT';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='RO';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='RU';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='SM';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='SI';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='ES';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='SE';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='CH';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='TR';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='UA';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='GB';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='US';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='UM';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='VA';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='IM';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='GG';</t>
+  </si>
+  <si>
+    <t>UPDATE oc_country set status='1' where iso_code_2='JE';</t>
   </si>
 </sst>
 </file>
@@ -1299,10 +1449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,9 +1460,10 @@
     <col min="1" max="1" width="50.5703125" customWidth="1"/>
     <col min="2" max="2" width="37.5703125" customWidth="1"/>
     <col min="6" max="6" width="56.140625" customWidth="1"/>
+    <col min="7" max="7" width="69.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>150</v>
       </c>
@@ -1332,8 +1483,11 @@
         <f>A1&amp;C1&amp;"'"&amp;E1</f>
         <v>UPDATE oc_country set status='1' where iso_code_2='AL';</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>150</v>
       </c>
@@ -1353,8 +1507,11 @@
         <f t="shared" ref="F2:F50" si="0">A2&amp;C2&amp;"'"&amp;E2</f>
         <v>UPDATE oc_country set status='1' where iso_code_2='AD';</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>150</v>
       </c>
@@ -1374,8 +1531,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='AM';</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>150</v>
       </c>
@@ -1395,8 +1555,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='AT';</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>150</v>
       </c>
@@ -1416,8 +1579,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='AZ';</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>150</v>
       </c>
@@ -1437,8 +1603,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='BY';</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>150</v>
       </c>
@@ -1458,8 +1627,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='BE';</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>150</v>
       </c>
@@ -1479,8 +1651,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='BA';</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>150</v>
       </c>
@@ -1500,8 +1675,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='BG';</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>150</v>
       </c>
@@ -1521,8 +1699,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='HR';</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>150</v>
       </c>
@@ -1542,8 +1723,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='CZ';</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>150</v>
       </c>
@@ -1563,8 +1747,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='DK';</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>150</v>
       </c>
@@ -1584,8 +1771,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='EE';</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>150</v>
       </c>
@@ -1605,8 +1795,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='FI';</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>150</v>
       </c>
@@ -1626,8 +1819,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='FR';</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>150</v>
       </c>
@@ -1647,8 +1843,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='GE';</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>150</v>
       </c>
@@ -1668,8 +1867,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='DE';</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>150</v>
       </c>
@@ -1689,8 +1891,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='GR';</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>150</v>
       </c>
@@ -1710,8 +1915,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='HU';</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>150</v>
       </c>
@@ -1731,8 +1939,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='IS';</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>150</v>
       </c>
@@ -1752,8 +1963,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='IE';</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>150</v>
       </c>
@@ -1773,8 +1987,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='IT';</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>150</v>
       </c>
@@ -1794,8 +2011,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='KZ';</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>150</v>
       </c>
@@ -1815,8 +2035,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='LV';</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>150</v>
       </c>
@@ -1836,8 +2059,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='LI';</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>150</v>
       </c>
@@ -1857,8 +2083,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='LT';</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>150</v>
       </c>
@@ -1878,8 +2107,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='LU';</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>150</v>
       </c>
@@ -1899,8 +2131,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='MT';</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>150</v>
       </c>
@@ -1920,8 +2155,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='MD';</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>150</v>
       </c>
@@ -1941,8 +2179,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='MC';</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>150</v>
       </c>
@@ -1962,8 +2203,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='NL';</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>150</v>
       </c>
@@ -1983,8 +2227,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='NO';</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>150</v>
       </c>
@@ -2004,8 +2251,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='PL';</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>150</v>
       </c>
@@ -2025,8 +2275,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='PT';</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>150</v>
       </c>
@@ -2046,8 +2299,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='RO';</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>150</v>
       </c>
@@ -2067,8 +2323,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='RU';</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>150</v>
       </c>
@@ -2088,8 +2347,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='SM';</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -2109,8 +2371,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='SI';</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>150</v>
       </c>
@@ -2130,8 +2395,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='ES';</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>150</v>
       </c>
@@ -2151,8 +2419,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='SE';</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>150</v>
       </c>
@@ -2172,8 +2443,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='CH';</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>150</v>
       </c>
@@ -2193,8 +2467,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='TR';</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>150</v>
       </c>
@@ -2214,8 +2491,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='UA';</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>150</v>
       </c>
@@ -2235,8 +2515,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='GB';</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>150</v>
       </c>
@@ -2256,8 +2539,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='US';</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>150</v>
       </c>
@@ -2277,8 +2563,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='UM';</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>150</v>
       </c>
@@ -2298,8 +2587,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='VA';</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>150</v>
       </c>
@@ -2319,8 +2611,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='IM';</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>150</v>
       </c>
@@ -2340,8 +2635,11 @@
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='GG';</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>150</v>
       </c>
@@ -2360,6 +2658,9 @@
       <c r="F50" t="str">
         <f t="shared" si="0"/>
         <v>UPDATE oc_country set status='1' where iso_code_2='JE';</v>
+      </c>
+      <c r="G50" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>